<commit_message>
[Document] Review Integration test
</commit_message>
<xml_diff>
--- a/Documentation/[FHF]_IntegrationTestCases.xlsx
+++ b/Documentation/[FHF]_IntegrationTestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\fu-house-finder\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B895A50-A1B7-4BC8-A427-312ED0859D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6B658D-E471-4BE0-B2AC-84CCB61F4A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -29,50 +29,17 @@
     <sheet name="(Staff) Change Password" sheetId="21" r:id="rId14"/>
     <sheet name="(Admin) Manage Account" sheetId="22" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4139" uniqueCount="1456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="1455">
   <si>
     <t>Project Name</t>
   </si>
@@ -9810,9 +9777,6 @@
   </si>
   <si>
     <t>TC_FHF_AddRoom_019</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>TS_FHF_ChangePassword_001</t>
@@ -10391,15 +10355,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10735,10 +10697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F30"/>
+  <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10809,10 +10771,10 @@
       <c r="B10" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="41" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -10823,10 +10785,10 @@
       <c r="B11" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="41" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -10837,10 +10799,10 @@
       <c r="B12" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="41" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -10851,10 +10813,10 @@
       <c r="B13" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="41" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -10865,10 +10827,10 @@
       <c r="B14" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="41" t="s">
         <v>354</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="41" t="s">
         <v>65</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -10879,10 +10841,10 @@
       <c r="B15" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="41" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -10893,10 +10855,10 @@
       <c r="B16" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="41" t="s">
         <v>354</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="41" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -10907,10 +10869,10 @@
       <c r="B17" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="41" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -10921,10 +10883,10 @@
       <c r="B18" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="41" t="s">
         <v>354</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="41" t="s">
         <v>65</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -10935,10 +10897,10 @@
       <c r="B19" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="41" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -10949,24 +10911,24 @@
       <c r="B20" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="41" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="16">
         <v>44907</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="41" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="11" t="s">
@@ -10977,10 +10939,10 @@
       <c r="B22" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="41" t="s">
         <v>61</v>
       </c>
       <c r="E22" s="11" t="s">
@@ -10991,10 +10953,10 @@
       <c r="B23" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="41" t="s">
         <v>61</v>
       </c>
       <c r="E23" s="11" t="s">
@@ -11002,44 +10964,18 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="13" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="16"/>
-      <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="16"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="17"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -11874,10 +11810,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11934,19 +11870,19 @@
         <v>342</v>
       </c>
       <c r="E3" s="14">
-        <f>COUNTIF(K8:K100,"Pass")</f>
+        <f>COUNTIF(K8:K93,"Pass")</f>
         <v>7</v>
       </c>
       <c r="F3" s="14">
-        <f>COUNTIF(K8:K100,"Fail")</f>
+        <f>COUNTIF(K8:K93,"Fail")</f>
         <v>0</v>
       </c>
       <c r="G3" s="14">
-        <f>COUNTIF(K8:K100,"Untested")</f>
+        <f>COUNTIF(K8:K93,"Untested")</f>
         <v>0</v>
       </c>
       <c r="H3" s="14">
-        <f>COUNTA(K8:K100)</f>
+        <f>COUNTA(K8:K93)</f>
         <v>7</v>
       </c>
     </row>
@@ -12315,196 +12251,84 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12513,10 +12337,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12573,19 +12397,19 @@
         <v>344</v>
       </c>
       <c r="E3" s="14">
-        <f>COUNTIF(K8:K36,"Pass")</f>
+        <f>COUNTIF(K8:K28,"Pass")</f>
         <v>21</v>
       </c>
       <c r="F3" s="14">
-        <f>COUNTIF(K8:K36,"Fail")</f>
+        <f>COUNTIF(K8:K28,"Fail")</f>
         <v>0</v>
       </c>
       <c r="G3" s="14">
-        <f>COUNTIF(K8:K36,"Untested")</f>
+        <f>COUNTIF(K8:K28,"Untested")</f>
         <v>0</v>
       </c>
       <c r="H3" s="14">
-        <f>COUNTA(K8:K36)</f>
+        <f>COUNTA(K8:K28)</f>
         <v>21</v>
       </c>
     </row>
@@ -13542,7 +13366,7 @@
       <c r="O27" s="24"/>
     </row>
     <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="21" t="s">
         <v>974</v>
       </c>
       <c r="B28" s="21" t="s">
@@ -13583,142 +13407,6 @@
         <v>40</v>
       </c>
       <c r="O28" s="24"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="24"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="24"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="24"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="24"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="24"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="24"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="24"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13727,10 +13415,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14157,118 +13845,6 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14276,10 +13852,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE30935E-E3A3-426A-BF9B-53B5FA0D8796}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14412,32 +13988,32 @@
     </row>
     <row r="8" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>1380</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="C8" s="21" t="s">
         <v>1381</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="21" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>1382</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>1381</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="21" t="s">
         <v>1383</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="21" t="s">
         <v>1384</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>1385</v>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="21" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="K8" s="26" t="s">
         <v>39</v>
@@ -14452,32 +14028,32 @@
     </row>
     <row r="9" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>1387</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="C9" s="21" t="s">
         <v>1388</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>1389</v>
-      </c>
       <c r="D9" s="21" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>1319</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="K9" s="26" t="s">
         <v>39</v>
@@ -14492,32 +14068,32 @@
     </row>
     <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>1392</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="C10" s="21" t="s">
         <v>1393</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>1394</v>
-      </c>
       <c r="D10" s="21" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>1324</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="K10" s="26" t="s">
         <v>39</v>
@@ -14532,32 +14108,32 @@
     </row>
     <row r="11" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>1396</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="C11" s="21" t="s">
         <v>1397</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>1398</v>
-      </c>
       <c r="D11" s="21" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>1329</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="K11" s="26" t="s">
         <v>39</v>
@@ -14572,25 +14148,25 @@
     </row>
     <row r="12" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>1400</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="C12" s="21" t="s">
         <v>1401</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="D12" s="21" t="s">
         <v>1402</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>1403</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>1334</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21" t="s">
@@ -14612,32 +14188,32 @@
     </row>
     <row r="13" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>1405</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="C13" s="21" t="s">
         <v>1406</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>1407</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>1408</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>1340</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="K13" s="26" t="s">
         <v>39</v>
@@ -14652,13 +14228,13 @@
     </row>
     <row r="14" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>1220</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>1220</v>
@@ -14668,7 +14244,7 @@
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21" t="s">
@@ -14687,40 +14263,6 @@
         <v>999</v>
       </c>
       <c r="N14" s="21"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="3" t="s">
-        <v>1379</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14730,10 +14272,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69627FBA-7EF3-4F8F-9D32-43D96E0E43AA}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14866,30 +14408,30 @@
     </row>
     <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>1412</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="D8" s="21" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>1414</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>1413</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>1414</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="21" t="s">
         <v>1415</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>1416</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="K8" s="26" t="s">
         <v>39</v>
@@ -14897,37 +14439,37 @@
       <c r="L8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="41" t="s">
+      <c r="M8" s="40" t="s">
         <v>335</v>
       </c>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="K9" s="26" t="s">
         <v>39</v>
@@ -14935,37 +14477,37 @@
       <c r="L9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="40" t="s">
         <v>335</v>
       </c>
       <c r="N9" s="21"/>
     </row>
     <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="K10" s="26" t="s">
         <v>39</v>
@@ -14973,39 +14515,39 @@
       <c r="L10" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="40" t="s">
         <v>335</v>
       </c>
       <c r="N10" s="21"/>
     </row>
     <row r="11" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="K11" s="26" t="s">
         <v>39</v>
@@ -15013,39 +14555,39 @@
       <c r="L11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="40" t="s">
         <v>335</v>
       </c>
       <c r="N11" s="21"/>
     </row>
     <row r="12" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="K12" s="26" t="s">
         <v>39</v>
@@ -15053,37 +14595,37 @@
       <c r="L12" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="41" t="s">
+      <c r="M12" s="40" t="s">
         <v>335</v>
       </c>
       <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="K13" s="26" t="s">
         <v>39</v>
@@ -15091,60 +14633,10 @@
       <c r="L13" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="40" t="s">
         <v>335</v>
       </c>
       <c r="N13" s="21"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="21"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="3" t="s">
-        <v>1379</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -15157,9 +14649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19607,8 +19097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3ACD261-CABF-419A-BC44-A08381E5AE9D}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19630,9 +19120,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e" cm="1">
-        <f t="array" ref="A1">A1:M21Module Name</f>
-        <v>#NAME?</v>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>64</v>
@@ -20670,7 +20159,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22106,8 +21595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22141,7 +21630,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>39</v>
@@ -22273,7 +21762,7 @@
       <c r="L8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N8" s="2"/>
@@ -22313,7 +21802,7 @@
       <c r="L9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="39" t="s">
+      <c r="M9" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N9" s="2"/>
@@ -22353,7 +21842,7 @@
       <c r="L10" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N10" s="2"/>
@@ -22393,7 +21882,7 @@
       <c r="L11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="39" t="s">
+      <c r="M11" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N11" s="2"/>
@@ -22433,7 +21922,7 @@
       <c r="L12" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="M12" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N12" s="2"/>
@@ -22473,7 +21962,7 @@
       <c r="L13" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="M13" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N13" s="2"/>
@@ -22513,7 +22002,7 @@
       <c r="L14" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N14" s="2"/>
@@ -22553,7 +22042,7 @@
       <c r="L15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="39" t="s">
+      <c r="M15" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N15" s="2"/>
@@ -22593,7 +22082,7 @@
       <c r="L16" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="39" t="s">
+      <c r="M16" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N16" s="2"/>
@@ -22633,7 +22122,7 @@
       <c r="L17" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M17" s="39" t="s">
+      <c r="M17" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N17" s="2"/>
@@ -22673,7 +22162,7 @@
       <c r="L18" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M18" s="39" t="s">
+      <c r="M18" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N18" s="2"/>
@@ -22711,7 +22200,7 @@
       <c r="L19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M19" s="39" t="s">
+      <c r="M19" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N19" s="2"/>
@@ -22749,7 +22238,7 @@
       <c r="L20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N20" s="2"/>
@@ -22787,7 +22276,7 @@
       <c r="L21" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M21" s="39" t="s">
+      <c r="M21" s="40" t="s">
         <v>337</v>
       </c>
       <c r="N21" s="2"/>
@@ -22827,9 +22316,10 @@
       <c r="L22" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="39" t="s">
+      <c r="M22" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" ht="315" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
@@ -22864,9 +22354,10 @@
       <c r="L23" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M23" s="39" t="s">
+      <c r="M23" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" ht="315" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
@@ -22903,9 +22394,10 @@
       <c r="L24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M24" s="39" t="s">
+      <c r="M24" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="345" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
@@ -22942,9 +22434,10 @@
       <c r="L25" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M25" s="39" t="s">
+      <c r="M25" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="315" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
@@ -22981,9 +22474,10 @@
       <c r="L26" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M26" s="39" t="s">
+      <c r="M26" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="315" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
@@ -23020,9 +22514,10 @@
       <c r="L27" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M27" s="39" t="s">
+      <c r="M27" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="315" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
@@ -23059,9 +22554,10 @@
       <c r="L28" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M28" s="39" t="s">
+      <c r="M28" s="40" t="s">
         <v>337</v>
       </c>
+      <c r="N28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23073,7 +22569,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23107,7 +22603,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>39</v>
@@ -23239,7 +22735,7 @@
       <c r="L8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="41" t="s">
+      <c r="M8" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N8" s="2"/>
@@ -23279,7 +22775,7 @@
       <c r="L9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N9" s="2"/>
@@ -23319,7 +22815,7 @@
       <c r="L10" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N10" s="2"/>
@@ -23359,7 +22855,7 @@
       <c r="L11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N11" s="2"/>
@@ -23399,7 +22895,7 @@
       <c r="L12" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="41" t="s">
+      <c r="M12" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N12" s="2"/>
@@ -23439,7 +22935,7 @@
       <c r="L13" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N13" s="2"/>
@@ -23479,7 +22975,7 @@
       <c r="L14" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N14" s="2"/>
@@ -23519,7 +23015,7 @@
       <c r="L15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N15" s="2"/>
@@ -23559,7 +23055,7 @@
       <c r="L16" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="41" t="s">
+      <c r="M16" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N16" s="2"/>
@@ -23599,7 +23095,7 @@
       <c r="L17" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="M17" s="39" t="s">
         <v>338</v>
       </c>
       <c r="N17" s="2"/>
@@ -23639,7 +23135,7 @@
       <c r="L18" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M18" s="41" t="s">
+      <c r="M18" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N18" s="2"/>
@@ -23679,7 +23175,7 @@
       <c r="L19" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M19" s="41" t="s">
+      <c r="M19" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N19" s="2"/>
@@ -23717,7 +23213,7 @@
       <c r="L20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="41" t="s">
+      <c r="M20" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N20" s="2"/>
@@ -23757,7 +23253,7 @@
       <c r="L21" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M21" s="41" t="s">
+      <c r="M21" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N21" s="2"/>
@@ -23797,7 +23293,7 @@
       <c r="L22" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="41" t="s">
+      <c r="M22" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N22" s="2"/>
@@ -23837,14 +23333,14 @@
       <c r="L23" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M23" s="41" t="s">
+      <c r="M23" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>1247</v>
@@ -23877,14 +23373,14 @@
       <c r="L24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M24" s="41" t="s">
+      <c r="M24" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>1253</v>
@@ -23917,14 +23413,14 @@
       <c r="L25" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M25" s="41" t="s">
+      <c r="M25" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>1258</v>
@@ -23957,14 +23453,14 @@
       <c r="L26" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M26" s="41" t="s">
+      <c r="M26" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>1264</v>
@@ -23997,14 +23493,14 @@
       <c r="L27" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M27" s="41" t="s">
+      <c r="M27" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B28" s="21" t="s">
         <v>1269</v>
@@ -24037,14 +23533,14 @@
       <c r="L28" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M28" s="41" t="s">
+      <c r="M28" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>1274</v>
@@ -24077,14 +23573,14 @@
       <c r="L29" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M29" s="41" t="s">
+      <c r="M29" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>1280</v>
@@ -24117,14 +23613,14 @@
       <c r="L30" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M30" s="41" t="s">
+      <c r="M30" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N30" s="2"/>
     </row>
     <row r="31" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>1286</v>
@@ -24157,14 +23653,14 @@
       <c r="L31" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M31" s="41" t="s">
+      <c r="M31" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N31" s="2"/>
     </row>
     <row r="32" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>1290</v>
@@ -24197,14 +23693,14 @@
       <c r="L32" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M32" s="41" t="s">
+      <c r="M32" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>1295</v>
@@ -24235,14 +23731,14 @@
       <c r="L33" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M33" s="41" t="s">
+      <c r="M33" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>1300</v>
@@ -24275,14 +23771,14 @@
       <c r="L34" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M34" s="41" t="s">
+      <c r="M34" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>1196</v>
@@ -24315,7 +23811,7 @@
       <c r="L35" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="M35" s="41" t="s">
+      <c r="M35" s="40" t="s">
         <v>338</v>
       </c>
       <c r="N35" s="2"/>

</xml_diff>